<commit_message>
some updates mon 22
</commit_message>
<xml_diff>
--- a/Project_info/Summery tables for report.xlsx
+++ b/Project_info/Summery tables for report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sylviabroadbent/Dropbox/Sylvia/UWA_Data_Analytics_Bootcamp/HOMEWORK/23 Project 3/Data-Analytics-Project-3/Project_info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{586952CE-7375-A048-8AF6-DCAACF9B3D1C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D39F137-D515-1B4C-9EC6-06225D609636}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25940" yWindow="-200" windowWidth="25600" windowHeight="28300" xr2:uid="{0BBD23A4-A283-624D-B6D4-A1A16531C452}"/>
+    <workbookView xWindow="-25940" yWindow="-260" windowWidth="25600" windowHeight="28300" xr2:uid="{0BBD23A4-A283-624D-B6D4-A1A16531C452}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="34">
   <si>
     <t>SMOKING</t>
   </si>
@@ -128,6 +128,15 @@
   <si>
     <t>random forest not reliable but still better than the relicable logistic regression?</t>
   </si>
+  <si>
+    <t>Model I would choose based on these outcomes</t>
+  </si>
+  <si>
+    <t>Models used for the website based on Github file size limit</t>
+  </si>
+  <si>
+    <t>&amp; because I ddin't save the RAW model</t>
+  </si>
 </sst>
 </file>
 
@@ -159,7 +168,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -178,8 +187,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="70">
+  <borders count="73">
     <border>
       <left/>
       <right/>
@@ -1074,11 +1089,56 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF003B46"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF003B46"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1113,73 +1173,18 @@
     <xf numFmtId="165" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="1" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1192,30 +1197,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1225,46 +1209,19 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1272,12 +1229,124 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="70" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="70" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="72" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1600,10 +1669,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA521345-460E-3447-B7BC-D9B25ACFAE5B}">
-  <dimension ref="A3:L85"/>
+  <dimension ref="A3:L92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K70" sqref="K70"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="L83" sqref="L83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1627,28 +1696,28 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
-      <c r="B4" s="92" t="s">
+      <c r="B4" s="86" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="93"/>
-      <c r="D4" s="28" t="s">
+      <c r="C4" s="87"/>
+      <c r="D4" s="90" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="29"/>
-      <c r="F4" s="30" t="s">
+      <c r="E4" s="91"/>
+      <c r="F4" s="92" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="30"/>
-      <c r="H4" s="28" t="s">
+      <c r="G4" s="92"/>
+      <c r="H4" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="29"/>
+      <c r="I4" s="91"/>
       <c r="J4" s="1"/>
     </row>
     <row r="5" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="94"/>
-      <c r="C5" s="95"/>
+      <c r="B5" s="88"/>
+      <c r="C5" s="89"/>
       <c r="D5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1671,7 +1740,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="93" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -1699,7 +1768,7 @@
     </row>
     <row r="7" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="35"/>
+      <c r="B7" s="94"/>
       <c r="C7" s="10" t="s">
         <v>6</v>
       </c>
@@ -1725,7 +1794,7 @@
     </row>
     <row r="8" spans="1:12" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="93" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="6" t="s">
@@ -1753,7 +1822,7 @@
     </row>
     <row r="9" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="27"/>
+      <c r="B9" s="95"/>
       <c r="C9" s="15" t="s">
         <v>6</v>
       </c>
@@ -1791,28 +1860,28 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
-      <c r="B11" s="92" t="s">
+      <c r="B11" s="86" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="93"/>
-      <c r="D11" s="28" t="s">
+      <c r="C11" s="87"/>
+      <c r="D11" s="90" t="s">
         <v>1</v>
       </c>
-      <c r="E11" s="29"/>
-      <c r="F11" s="30" t="s">
+      <c r="E11" s="91"/>
+      <c r="F11" s="92" t="s">
         <v>2</v>
       </c>
-      <c r="G11" s="30"/>
-      <c r="H11" s="28" t="s">
+      <c r="G11" s="92"/>
+      <c r="H11" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="I11" s="29"/>
+      <c r="I11" s="91"/>
       <c r="J11" s="1"/>
     </row>
     <row r="12" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="94"/>
-      <c r="C12" s="95"/>
+      <c r="B12" s="88"/>
+      <c r="C12" s="89"/>
       <c r="D12" s="2" t="s">
         <v>7</v>
       </c>
@@ -1835,7 +1904,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
-      <c r="B13" s="26" t="s">
+      <c r="B13" s="93" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="6" t="s">
@@ -1847,7 +1916,7 @@
       <c r="E13" s="8">
         <v>0.54213599999999995</v>
       </c>
-      <c r="F13" s="40">
+      <c r="F13" s="26">
         <v>0.54042999999999997</v>
       </c>
       <c r="G13" s="6">
@@ -1863,7 +1932,7 @@
     </row>
     <row r="14" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
-      <c r="B14" s="35"/>
+      <c r="B14" s="94"/>
       <c r="C14" s="10" t="s">
         <v>6</v>
       </c>
@@ -1889,7 +1958,7 @@
     </row>
     <row r="15" spans="1:12" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
-      <c r="B15" s="26" t="s">
+      <c r="B15" s="93" t="s">
         <v>4</v>
       </c>
       <c r="C15" s="6" t="s">
@@ -1917,7 +1986,7 @@
     </row>
     <row r="16" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="27"/>
+      <c r="B16" s="95"/>
       <c r="C16" s="15" t="s">
         <v>6</v>
       </c>
@@ -1943,40 +2012,40 @@
     </row>
     <row r="17" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="B17" s="63"/>
-      <c r="C17" s="64"/>
-      <c r="D17" s="64"/>
-      <c r="E17" s="64"/>
-      <c r="F17" s="64"/>
-      <c r="G17" s="64"/>
-      <c r="H17" s="64"/>
-      <c r="I17" s="64"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="45"/>
+      <c r="I17" s="45"/>
       <c r="J17" s="1"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
-      <c r="B18" s="92" t="s">
+      <c r="B18" s="86" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="93"/>
-      <c r="D18" s="28" t="s">
+      <c r="C18" s="87"/>
+      <c r="D18" s="90" t="s">
         <v>1</v>
       </c>
-      <c r="E18" s="29"/>
-      <c r="F18" s="30" t="s">
+      <c r="E18" s="91"/>
+      <c r="F18" s="92" t="s">
         <v>2</v>
       </c>
-      <c r="G18" s="30"/>
-      <c r="H18" s="28" t="s">
+      <c r="G18" s="92"/>
+      <c r="H18" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="I18" s="29"/>
+      <c r="I18" s="91"/>
       <c r="J18" s="1"/>
     </row>
     <row r="19" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="94"/>
-      <c r="C19" s="95"/>
+      <c r="B19" s="88"/>
+      <c r="C19" s="89"/>
       <c r="D19" s="2" t="s">
         <v>7</v>
       </c>
@@ -1999,7 +2068,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
-      <c r="B20" s="26" t="s">
+      <c r="B20" s="93" t="s">
         <v>11</v>
       </c>
       <c r="C20" s="6" t="s">
@@ -2011,10 +2080,10 @@
       <c r="E20" s="8">
         <v>0.92258300000000004</v>
       </c>
-      <c r="F20" s="31" t="s">
+      <c r="F20" s="107" t="s">
         <v>12</v>
       </c>
-      <c r="G20" s="32"/>
+      <c r="G20" s="108"/>
       <c r="H20" s="7">
         <v>0.922018</v>
       </c>
@@ -2025,7 +2094,7 @@
     </row>
     <row r="21" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
-      <c r="B21" s="35"/>
+      <c r="B21" s="94"/>
       <c r="C21" s="10" t="s">
         <v>6</v>
       </c>
@@ -2035,8 +2104,8 @@
       <c r="E21" s="12">
         <v>0.92082200000000003</v>
       </c>
-      <c r="F21" s="33"/>
-      <c r="G21" s="34"/>
+      <c r="F21" s="109"/>
+      <c r="G21" s="110"/>
       <c r="H21" s="14">
         <v>0.91990000000000005</v>
       </c>
@@ -2047,7 +2116,7 @@
     </row>
     <row r="22" spans="1:11" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
-      <c r="B22" s="26" t="s">
+      <c r="B22" s="93" t="s">
         <v>4</v>
       </c>
       <c r="C22" s="6" t="s">
@@ -2059,11 +2128,11 @@
       <c r="E22" s="8">
         <v>0.99874399999999997</v>
       </c>
-      <c r="F22" s="36" t="s">
+      <c r="F22" s="103" t="s">
         <v>12</v>
       </c>
-      <c r="G22" s="37"/>
-      <c r="H22" s="58">
+      <c r="G22" s="104"/>
+      <c r="H22" s="39">
         <v>0.99228000000000005</v>
       </c>
       <c r="I22" s="22">
@@ -2073,7 +2142,7 @@
     </row>
     <row r="23" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="27"/>
+      <c r="B23" s="95"/>
       <c r="C23" s="15" t="s">
         <v>6</v>
       </c>
@@ -2083,8 +2152,8 @@
       <c r="E23" s="25">
         <v>0.91980799999999996</v>
       </c>
-      <c r="F23" s="38"/>
-      <c r="G23" s="39"/>
+      <c r="F23" s="105"/>
+      <c r="G23" s="106"/>
       <c r="H23" s="16">
         <v>0.91561400000000004</v>
       </c>
@@ -2107,29 +2176,29 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
-      <c r="B25" s="92" t="s">
+      <c r="B25" s="86" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="93"/>
-      <c r="D25" s="28" t="s">
+      <c r="C25" s="87"/>
+      <c r="D25" s="90" t="s">
         <v>27</v>
       </c>
-      <c r="E25" s="29"/>
-      <c r="F25" s="30" t="s">
+      <c r="E25" s="91"/>
+      <c r="F25" s="92" t="s">
         <v>15</v>
       </c>
-      <c r="G25" s="30"/>
-      <c r="H25" s="28" t="s">
+      <c r="G25" s="92"/>
+      <c r="H25" s="90" t="s">
         <v>28</v>
       </c>
-      <c r="I25" s="29"/>
-      <c r="J25" s="64"/>
-      <c r="K25" s="64"/>
+      <c r="I25" s="91"/>
+      <c r="J25" s="45"/>
+      <c r="K25" s="45"/>
     </row>
     <row r="26" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
-      <c r="B26" s="94"/>
-      <c r="C26" s="95"/>
+      <c r="B26" s="88"/>
+      <c r="C26" s="89"/>
       <c r="D26" s="2" t="s">
         <v>7</v>
       </c>
@@ -2148,12 +2217,12 @@
       <c r="I26" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J26" s="64"/>
-      <c r="K26" s="64"/>
+      <c r="J26" s="45"/>
+      <c r="K26" s="45"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
-      <c r="B27" s="26" t="s">
+      <c r="B27" s="93" t="s">
         <v>11</v>
       </c>
       <c r="C27" s="6" t="s">
@@ -2162,7 +2231,7 @@
       <c r="D27" s="23">
         <v>1</v>
       </c>
-      <c r="E27" s="60">
+      <c r="E27" s="41">
         <v>1</v>
       </c>
       <c r="F27" s="7">
@@ -2177,16 +2246,16 @@
       <c r="I27" s="8">
         <v>0.90949400000000002</v>
       </c>
-      <c r="J27" s="64"/>
-      <c r="K27" s="64"/>
+      <c r="J27" s="45"/>
+      <c r="K27" s="45"/>
     </row>
     <row r="28" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
-      <c r="B28" s="35"/>
+      <c r="B28" s="94"/>
       <c r="C28" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D28" s="59">
+      <c r="D28" s="40">
         <v>1</v>
       </c>
       <c r="E28" s="12">
@@ -2204,12 +2273,12 @@
       <c r="I28" s="12">
         <v>0.91496900000000003</v>
       </c>
-      <c r="J28" s="64"/>
-      <c r="K28" s="64"/>
+      <c r="J28" s="45"/>
+      <c r="K28" s="45"/>
     </row>
     <row r="29" spans="1:11" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
-      <c r="B29" s="26" t="s">
+      <c r="B29" s="93" t="s">
         <v>4</v>
       </c>
       <c r="C29" s="6" t="s">
@@ -2218,10 +2287,10 @@
       <c r="D29" s="23">
         <v>1</v>
       </c>
-      <c r="E29" s="60">
+      <c r="E29" s="41">
         <v>1</v>
       </c>
-      <c r="F29" s="58">
+      <c r="F29" s="39">
         <v>0.99992999999999999</v>
       </c>
       <c r="G29" s="22">
@@ -2233,19 +2302,19 @@
       <c r="I29" s="8">
         <v>0.99980400000000003</v>
       </c>
-      <c r="J29" s="64"/>
-      <c r="K29" s="64"/>
+      <c r="J29" s="45"/>
+      <c r="K29" s="45"/>
     </row>
     <row r="30" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
-      <c r="B30" s="27"/>
+      <c r="B30" s="95"/>
       <c r="C30" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D30" s="59">
+      <c r="D30" s="40">
         <v>1</v>
       </c>
-      <c r="E30" s="62">
+      <c r="E30" s="43">
         <v>1</v>
       </c>
       <c r="F30" s="24">
@@ -2260,46 +2329,46 @@
       <c r="I30" s="17">
         <v>0.91381599999999996</v>
       </c>
-      <c r="J30" s="64"/>
-      <c r="K30" s="64"/>
+      <c r="J30" s="45"/>
+      <c r="K30" s="45"/>
     </row>
     <row r="31" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
-      <c r="B31" s="63"/>
-      <c r="C31" s="64"/>
-      <c r="D31" s="65"/>
-      <c r="E31" s="65"/>
-      <c r="F31" s="66"/>
-      <c r="G31" s="64"/>
-      <c r="H31" s="64"/>
-      <c r="I31" s="64"/>
-      <c r="J31" s="64"/>
-      <c r="K31" s="64"/>
+      <c r="B31" s="44"/>
+      <c r="C31" s="45"/>
+      <c r="D31" s="46"/>
+      <c r="E31" s="46"/>
+      <c r="F31" s="47"/>
+      <c r="G31" s="45"/>
+      <c r="H31" s="45"/>
+      <c r="I31" s="45"/>
+      <c r="J31" s="45"/>
+      <c r="K31" s="45"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
-      <c r="B32" s="92" t="s">
+      <c r="B32" s="86" t="s">
         <v>26</v>
       </c>
-      <c r="C32" s="93"/>
-      <c r="D32" s="28" t="s">
+      <c r="C32" s="87"/>
+      <c r="D32" s="90" t="s">
         <v>27</v>
       </c>
-      <c r="E32" s="29"/>
-      <c r="F32" s="30" t="s">
+      <c r="E32" s="91"/>
+      <c r="F32" s="92" t="s">
         <v>15</v>
       </c>
-      <c r="G32" s="30"/>
-      <c r="H32" s="28" t="s">
+      <c r="G32" s="92"/>
+      <c r="H32" s="90" t="s">
         <v>29</v>
       </c>
-      <c r="I32" s="29"/>
+      <c r="I32" s="91"/>
       <c r="J32" s="1"/>
     </row>
     <row r="33" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
-      <c r="B33" s="94"/>
-      <c r="C33" s="95"/>
+      <c r="B33" s="88"/>
+      <c r="C33" s="89"/>
       <c r="D33" s="2" t="s">
         <v>7</v>
       </c>
@@ -2322,13 +2391,13 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
-      <c r="B34" s="26" t="s">
+      <c r="B34" s="93" t="s">
         <v>11</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D34" s="58">
+      <c r="D34" s="39">
         <v>0.72318199999999999</v>
       </c>
       <c r="E34" s="22">
@@ -2340,7 +2409,7 @@
       <c r="G34" s="8">
         <v>0.88727900000000004</v>
       </c>
-      <c r="H34" s="58">
+      <c r="H34" s="39">
         <v>0.90961999999999998</v>
       </c>
       <c r="I34" s="22">
@@ -2350,14 +2419,14 @@
     </row>
     <row r="35" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
-      <c r="B35" s="35"/>
+      <c r="B35" s="94"/>
       <c r="C35" s="10" t="s">
         <v>6</v>
       </c>
       <c r="D35" s="14">
         <v>0.72034200000000004</v>
       </c>
-      <c r="E35" s="61">
+      <c r="E35" s="42">
         <v>0.72024999999999995</v>
       </c>
       <c r="F35" s="14">
@@ -2376,25 +2445,25 @@
     </row>
     <row r="36" spans="1:12" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
-      <c r="B36" s="26" t="s">
+      <c r="B36" s="93" t="s">
         <v>4</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D36" s="58">
+      <c r="D36" s="39">
         <v>0.930844</v>
       </c>
       <c r="E36" s="22">
         <v>0.930844</v>
       </c>
-      <c r="F36" s="58">
+      <c r="F36" s="39">
         <v>0.97364899999999999</v>
       </c>
       <c r="G36" s="22">
         <v>0.97364899999999999</v>
       </c>
-      <c r="H36" s="58">
+      <c r="H36" s="39">
         <v>0.97472000000000003</v>
       </c>
       <c r="I36" s="22">
@@ -2404,14 +2473,14 @@
     </row>
     <row r="37" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
-      <c r="B37" s="27"/>
+      <c r="B37" s="95"/>
       <c r="C37" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D37" s="14">
+      <c r="D37" s="113">
         <v>0.71919</v>
       </c>
-      <c r="E37" s="61">
+      <c r="E37" s="114">
         <v>0.71389000000000002</v>
       </c>
       <c r="F37" s="24">
@@ -2464,8 +2533,8 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
-      <c r="J44" s="45"/>
-      <c r="K44" s="45"/>
+      <c r="J44" s="30"/>
+      <c r="K44" s="30"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
@@ -2477,8 +2546,8 @@
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
-      <c r="J45" s="45"/>
-      <c r="K45" s="45"/>
+      <c r="J45" s="30"/>
+      <c r="K45" s="30"/>
       <c r="L45" s="1"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
@@ -2494,75 +2563,75 @@
       <c r="L46" s="1"/>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A50" s="45"/>
-      <c r="B50" s="45"/>
-      <c r="C50" s="45"/>
-      <c r="D50" s="45"/>
-      <c r="E50" s="45"/>
-      <c r="F50" s="45"/>
-      <c r="G50" s="45"/>
-      <c r="H50" s="45"/>
-      <c r="I50" s="45"/>
-      <c r="L50" s="45"/>
+      <c r="A50" s="30"/>
+      <c r="B50" s="30"/>
+      <c r="C50" s="30"/>
+      <c r="D50" s="30"/>
+      <c r="E50" s="30"/>
+      <c r="F50" s="30"/>
+      <c r="G50" s="30"/>
+      <c r="H50" s="30"/>
+      <c r="I50" s="30"/>
+      <c r="L50" s="30"/>
     </row>
     <row r="51" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="45"/>
-      <c r="B51" s="45"/>
-      <c r="C51" s="45"/>
-      <c r="D51" s="45"/>
-      <c r="E51" s="45"/>
-      <c r="F51" s="45"/>
-      <c r="G51" s="45"/>
-      <c r="H51" s="45"/>
-      <c r="I51" s="45"/>
-      <c r="L51" s="45"/>
+      <c r="A51" s="30"/>
+      <c r="B51" s="30"/>
+      <c r="C51" s="30"/>
+      <c r="D51" s="30"/>
+      <c r="E51" s="30"/>
+      <c r="F51" s="30"/>
+      <c r="G51" s="30"/>
+      <c r="H51" s="30"/>
+      <c r="I51" s="30"/>
+      <c r="L51" s="30"/>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A52" s="45"/>
+      <c r="A52" s="30"/>
       <c r="B52" s="96" t="s">
         <v>13</v>
       </c>
       <c r="C52" s="97"/>
-      <c r="D52" s="67" t="s">
+      <c r="D52" s="99" t="s">
         <v>11</v>
       </c>
-      <c r="E52" s="68"/>
-      <c r="F52" s="89" t="s">
+      <c r="E52" s="100"/>
+      <c r="F52" s="101" t="s">
         <v>4</v>
       </c>
-      <c r="G52" s="69"/>
+      <c r="G52" s="102"/>
       <c r="H52" s="1"/>
     </row>
     <row r="53" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="45"/>
+      <c r="A53" s="30"/>
       <c r="B53" s="98"/>
-      <c r="C53" s="95"/>
+      <c r="C53" s="89"/>
       <c r="D53" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E53" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F53" s="90" t="s">
+      <c r="F53" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="G53" s="91" t="s">
+      <c r="G53" s="63" t="s">
         <v>8</v>
       </c>
       <c r="H53" s="1"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A54" s="45"/>
-      <c r="B54" s="70" t="s">
+      <c r="A54" s="30"/>
+      <c r="B54" s="82" t="s">
         <v>0</v>
       </c>
       <c r="C54" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D54" s="100">
+      <c r="D54" s="65">
         <v>0.99935399999999996</v>
       </c>
-      <c r="E54" s="8">
+      <c r="E54" s="119">
         <v>0.99935399999999996</v>
       </c>
       <c r="F54" s="7">
@@ -2574,44 +2643,44 @@
       <c r="H54" s="1"/>
     </row>
     <row r="55" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="45"/>
-      <c r="B55" s="72"/>
+      <c r="A55" s="30"/>
+      <c r="B55" s="83"/>
       <c r="C55" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D55" s="101">
+      <c r="D55" s="66">
         <v>0.99939999999999996</v>
       </c>
-      <c r="E55" s="61">
+      <c r="E55" s="125">
         <v>0.99939999999999996</v>
       </c>
-      <c r="F55" s="51">
+      <c r="F55" s="34">
         <v>0.99935399999999996</v>
       </c>
-      <c r="G55" s="52">
+      <c r="G55" s="35">
         <v>0.99921599999999999</v>
       </c>
       <c r="H55" s="1"/>
     </row>
     <row r="56" spans="1:12" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="45"/>
-      <c r="B56" s="74" t="s">
+      <c r="A56" s="30"/>
+      <c r="B56" s="84" t="s">
         <v>9</v>
       </c>
-      <c r="C56" s="41" t="s">
+      <c r="C56" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D56" s="42">
+      <c r="D56" s="123">
         <v>0.378361</v>
       </c>
-      <c r="E56" s="43">
-        <v>0.37883299999999998</v>
-      </c>
-      <c r="F56" s="102">
-        <v>0.87316499999999997</v>
-      </c>
-      <c r="G56" s="75">
-        <v>0.87316499999999997</v>
+      <c r="E56" s="121">
+        <v>0.37816499999999997</v>
+      </c>
+      <c r="F56" s="29">
+        <v>0.91788199999999998</v>
+      </c>
+      <c r="G56" s="50">
+        <v>0.91788199999999998</v>
       </c>
       <c r="H56" s="1"/>
       <c r="I56" s="1" t="s">
@@ -2619,154 +2688,154 @@
       </c>
     </row>
     <row r="57" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="45"/>
-      <c r="B57" s="76"/>
-      <c r="C57" s="50" t="s">
+      <c r="A57" s="30"/>
+      <c r="B57" s="85"/>
+      <c r="C57" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="D57" s="51">
+      <c r="D57" s="124">
         <v>0.37238399999999999</v>
       </c>
-      <c r="E57" s="52">
-        <v>0.372614</v>
-      </c>
-      <c r="F57" s="103">
-        <v>0.47525099999999998</v>
-      </c>
-      <c r="G57" s="77">
-        <v>0.47225499999999998</v>
+      <c r="E57" s="122">
+        <v>0.37196899999999999</v>
+      </c>
+      <c r="F57" s="36">
+        <v>0.473223</v>
+      </c>
+      <c r="G57" s="51">
+        <v>0.47207100000000002</v>
       </c>
       <c r="H57" s="1"/>
     </row>
     <row r="58" spans="1:12" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="45"/>
-      <c r="B58" s="54" t="s">
+      <c r="A58" s="30"/>
+      <c r="B58" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="C58" s="55" t="s">
+      <c r="C58" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="D58" s="78">
+      <c r="D58" s="52">
         <v>0.92019799999999996</v>
       </c>
-      <c r="E58" s="104">
+      <c r="E58" s="115">
         <v>0.92040500000000003</v>
       </c>
-      <c r="F58" s="80">
+      <c r="F58" s="54">
         <v>0.99142699999999995</v>
       </c>
-      <c r="G58" s="79">
+      <c r="G58" s="53">
         <v>0.99142699999999995</v>
       </c>
       <c r="H58" s="1"/>
     </row>
     <row r="59" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="45"/>
-      <c r="B59" s="56"/>
-      <c r="C59" s="57" t="s">
+      <c r="A59" s="30"/>
+      <c r="B59" s="81"/>
+      <c r="C59" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="D59" s="88">
+      <c r="D59" s="61">
         <v>0.91754999999999998</v>
       </c>
-      <c r="E59" s="105">
+      <c r="E59" s="116">
         <v>0.91773400000000005</v>
       </c>
-      <c r="F59" s="83">
+      <c r="F59" s="57">
         <v>0.91312499999999996</v>
       </c>
-      <c r="G59" s="82">
+      <c r="G59" s="56">
         <v>0.91192700000000004</v>
       </c>
       <c r="H59" s="1"/>
     </row>
     <row r="60" spans="1:12" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="45"/>
-      <c r="B60" s="54" t="s">
+      <c r="A60" s="30"/>
+      <c r="B60" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="C60" s="55" t="s">
+      <c r="C60" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="D60" s="78">
+      <c r="D60" s="52">
         <v>0.72340099999999996</v>
       </c>
-      <c r="E60" s="104">
+      <c r="E60" s="115">
         <v>0.72335499999999997</v>
       </c>
-      <c r="F60" s="80">
+      <c r="F60" s="54">
         <v>0.95303599999999999</v>
       </c>
-      <c r="G60" s="79">
+      <c r="G60" s="53">
         <v>0.95303599999999999</v>
       </c>
       <c r="H60" s="1"/>
     </row>
     <row r="61" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="45"/>
-      <c r="B61" s="56"/>
-      <c r="C61" s="57" t="s">
+      <c r="A61" s="30"/>
+      <c r="B61" s="81"/>
+      <c r="C61" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="D61" s="81">
+      <c r="D61" s="55">
         <v>0.72089499999999995</v>
       </c>
-      <c r="E61" s="105">
+      <c r="E61" s="116">
         <v>0.72117200000000004</v>
       </c>
-      <c r="F61" s="106">
+      <c r="F61" s="69">
         <v>0.72024999999999995</v>
       </c>
-      <c r="G61" s="82">
+      <c r="G61" s="56">
         <v>0.71637899999999999</v>
       </c>
       <c r="H61" s="1"/>
     </row>
     <row r="62" spans="1:12" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="45"/>
-      <c r="B62" s="54" t="s">
+      <c r="A62" s="30"/>
+      <c r="B62" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="C62" s="55" t="s">
+      <c r="C62" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="D62" s="107">
+      <c r="D62" s="70">
         <v>0.887602</v>
       </c>
-      <c r="E62" s="78">
+      <c r="E62" s="117">
         <v>0.887602</v>
       </c>
-      <c r="F62" s="80">
+      <c r="F62" s="54">
         <v>0.98763599999999996</v>
       </c>
-      <c r="G62" s="79">
+      <c r="G62" s="53">
         <v>0.98763599999999996</v>
       </c>
       <c r="H62" s="1"/>
     </row>
     <row r="63" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="45"/>
-      <c r="B63" s="56"/>
-      <c r="C63" s="57" t="s">
+      <c r="A63" s="30"/>
+      <c r="B63" s="81"/>
+      <c r="C63" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="D63" s="108">
+      <c r="D63" s="71">
         <v>0.890266</v>
       </c>
-      <c r="E63" s="81">
+      <c r="E63" s="118">
         <v>0.890266</v>
       </c>
-      <c r="F63" s="83">
+      <c r="F63" s="57">
         <v>0.88123300000000004</v>
       </c>
-      <c r="G63" s="82">
+      <c r="G63" s="56">
         <v>0.87754600000000005</v>
       </c>
       <c r="H63" s="1"/>
     </row>
     <row r="64" spans="1:12" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="45"/>
-      <c r="B64" s="70" t="s">
+      <c r="A64" s="30"/>
+      <c r="B64" s="82" t="s">
         <v>16</v>
       </c>
       <c r="C64" s="6" t="s">
@@ -2775,369 +2844,369 @@
       <c r="D64" s="7">
         <v>0.98300399999999999</v>
       </c>
-      <c r="E64" s="8">
+      <c r="E64" s="119">
         <v>0.98300399999999999</v>
       </c>
-      <c r="F64" s="109">
+      <c r="F64" s="72">
         <v>0.99848999999999999</v>
       </c>
-      <c r="G64" s="99">
+      <c r="G64" s="64">
         <v>0.99848999999999999</v>
       </c>
       <c r="H64" s="1"/>
     </row>
     <row r="65" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
-      <c r="B65" s="72"/>
+      <c r="B65" s="83"/>
       <c r="C65" s="10" t="s">
         <v>6</v>
       </c>
       <c r="D65" s="11">
         <v>0.98391499999999998</v>
       </c>
-      <c r="E65" s="12">
+      <c r="E65" s="120">
         <v>0.98391499999999998</v>
       </c>
-      <c r="F65" s="110">
+      <c r="F65" s="73">
         <v>0.98308499999999999</v>
       </c>
-      <c r="G65" s="73">
+      <c r="G65" s="49">
         <v>0.98285500000000003</v>
       </c>
       <c r="H65" s="1"/>
     </row>
     <row r="66" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1"/>
-      <c r="B66" s="74" t="s">
+      <c r="B66" s="84" t="s">
         <v>17</v>
       </c>
-      <c r="C66" s="41" t="s">
+      <c r="C66" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D66" s="42">
+      <c r="D66" s="28">
         <v>0.99142699999999995</v>
       </c>
-      <c r="E66" s="43">
+      <c r="E66" s="121">
         <v>0.99142699999999995</v>
       </c>
-      <c r="F66" s="102">
+      <c r="F66" s="67">
         <v>0.99942299999999995</v>
       </c>
-      <c r="G66" s="75">
+      <c r="G66" s="50">
         <v>0.99942299999999995</v>
       </c>
       <c r="H66" s="1"/>
     </row>
     <row r="67" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
-      <c r="B67" s="76"/>
-      <c r="C67" s="50" t="s">
+      <c r="B67" s="85"/>
+      <c r="C67" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="D67" s="51">
+      <c r="D67" s="34">
         <v>0.991842</v>
       </c>
-      <c r="E67" s="52">
+      <c r="E67" s="122">
         <v>0.991842</v>
       </c>
-      <c r="F67" s="103">
+      <c r="F67" s="68">
         <v>0.99147300000000005</v>
       </c>
-      <c r="G67" s="77">
+      <c r="G67" s="51">
         <v>0.99142699999999995</v>
       </c>
       <c r="H67" s="1"/>
     </row>
     <row r="68" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1"/>
-      <c r="B68" s="54" t="s">
+      <c r="B68" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="C68" s="55" t="s">
+      <c r="C68" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="D68" s="107">
+      <c r="D68" s="70">
         <v>0.96610200000000002</v>
       </c>
-      <c r="E68" s="79">
+      <c r="E68" s="115">
         <v>0.96610200000000002</v>
       </c>
-      <c r="F68" s="80">
+      <c r="F68" s="54">
         <v>0.99662399999999995</v>
       </c>
-      <c r="G68" s="79">
+      <c r="G68" s="53">
         <v>0.99662399999999995</v>
       </c>
       <c r="H68" s="1"/>
     </row>
     <row r="69" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
-      <c r="B69" s="56"/>
-      <c r="C69" s="57" t="s">
+      <c r="B69" s="81"/>
+      <c r="C69" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="D69" s="108">
+      <c r="D69" s="71">
         <v>0.96644799999999997</v>
       </c>
-      <c r="E69" s="82">
+      <c r="E69" s="116">
         <v>0.96644799999999997</v>
       </c>
-      <c r="F69" s="106">
+      <c r="F69" s="69">
         <v>0.96442000000000005</v>
       </c>
-      <c r="G69" s="82">
+      <c r="G69" s="56">
         <v>0.96340599999999998</v>
       </c>
       <c r="H69" s="1"/>
     </row>
     <row r="70" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1"/>
-      <c r="B70" s="54" t="s">
+      <c r="B70" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="C70" s="55" t="s">
+      <c r="C70" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="D70" s="107">
+      <c r="D70" s="70">
         <v>0.66734599999999999</v>
       </c>
-      <c r="E70" s="79">
+      <c r="E70" s="115">
         <v>0.66751899999999997</v>
       </c>
-      <c r="F70" s="80">
+      <c r="F70" s="54">
         <v>0.93794200000000005</v>
       </c>
-      <c r="G70" s="79">
+      <c r="G70" s="53">
         <v>0.93794200000000005</v>
       </c>
       <c r="H70" s="1"/>
     </row>
     <row r="71" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
-      <c r="B71" s="56"/>
-      <c r="C71" s="57" t="s">
+      <c r="B71" s="81"/>
+      <c r="C71" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="D71" s="108">
+      <c r="D71" s="71">
         <v>0.66522199999999998</v>
       </c>
-      <c r="E71" s="82">
+      <c r="E71" s="116">
         <v>0.66448499999999999</v>
       </c>
-      <c r="F71" s="106">
+      <c r="F71" s="69">
         <v>0.64097999999999999</v>
       </c>
-      <c r="G71" s="82">
+      <c r="G71" s="56">
         <v>0.63738499999999998</v>
       </c>
       <c r="H71" s="1"/>
     </row>
     <row r="72" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A72" s="1"/>
-      <c r="B72" s="54" t="s">
+      <c r="B72" s="80" t="s">
         <v>20</v>
       </c>
-      <c r="C72" s="55" t="s">
+      <c r="C72" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="D72" s="107">
+      <c r="D72" s="70">
         <v>0.80465399999999998</v>
       </c>
-      <c r="E72" s="79">
+      <c r="E72" s="115">
         <v>0.80290300000000003</v>
       </c>
-      <c r="F72" s="80">
+      <c r="F72" s="54">
         <v>0.96504199999999996</v>
       </c>
-      <c r="G72" s="79">
+      <c r="G72" s="53">
         <v>0.96504199999999996</v>
       </c>
       <c r="H72" s="1"/>
     </row>
     <row r="73" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
-      <c r="B73" s="56"/>
-      <c r="C73" s="57" t="s">
+      <c r="B73" s="81"/>
+      <c r="C73" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="D73" s="108">
+      <c r="D73" s="71">
         <v>0.80680200000000002</v>
       </c>
-      <c r="E73" s="82">
+      <c r="E73" s="116">
         <v>0.80495799999999995</v>
       </c>
-      <c r="F73" s="83">
+      <c r="F73" s="57">
         <v>0.78928900000000002</v>
       </c>
-      <c r="G73" s="82">
+      <c r="G73" s="56">
         <v>0.78348229999999996</v>
       </c>
       <c r="H73" s="1"/>
     </row>
     <row r="74" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A74" s="1"/>
-      <c r="B74" s="70" t="s">
+      <c r="B74" s="82" t="s">
         <v>21</v>
       </c>
       <c r="C74" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D74" s="58">
+      <c r="D74" s="39">
         <v>0.86419999999999997</v>
       </c>
-      <c r="E74" s="113">
-        <v>0.88727900000000004</v>
-      </c>
-      <c r="F74" s="40">
-        <v>0.97364899999999999</v>
-      </c>
-      <c r="G74" s="71">
-        <v>0.97364899999999999</v>
+      <c r="E74" s="119">
+        <v>0.86431599999999997</v>
+      </c>
+      <c r="F74" s="26">
+        <v>0.979375</v>
+      </c>
+      <c r="G74" s="48">
+        <v>0.979375</v>
       </c>
       <c r="H74" s="1"/>
     </row>
     <row r="75" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
-      <c r="B75" s="72"/>
+      <c r="B75" s="83"/>
       <c r="C75" s="10" t="s">
         <v>6</v>
       </c>
       <c r="D75" s="11">
         <v>0.86630099999999999</v>
       </c>
-      <c r="E75" s="114">
-        <v>0.88966699999999999</v>
+      <c r="E75" s="120">
+        <v>0.86666900000000002</v>
       </c>
       <c r="F75" s="20">
-        <v>0.87773000000000001</v>
-      </c>
-      <c r="G75" s="73">
-        <v>0.87487300000000001</v>
+        <v>0.85270500000000005</v>
+      </c>
+      <c r="G75" s="49">
+        <v>0.84846500000000002</v>
       </c>
       <c r="H75" s="1"/>
     </row>
     <row r="76" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A76" s="1"/>
-      <c r="B76" s="74" t="s">
+      <c r="B76" s="84" t="s">
         <v>22</v>
       </c>
-      <c r="C76" s="41" t="s">
+      <c r="C76" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D76" s="42">
+      <c r="D76" s="28">
         <v>0.88769399999999998</v>
       </c>
-      <c r="E76" s="115">
+      <c r="E76" s="121">
         <v>0.88771699999999998</v>
       </c>
-      <c r="F76" s="44">
+      <c r="F76" s="29">
         <v>0.97863800000000001</v>
       </c>
-      <c r="G76" s="75">
+      <c r="G76" s="50">
         <v>0.97863800000000001</v>
       </c>
       <c r="H76" s="1"/>
     </row>
     <row r="77" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
-      <c r="B77" s="76"/>
-      <c r="C77" s="50" t="s">
+      <c r="B77" s="85"/>
+      <c r="C77" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="D77" s="112">
+      <c r="D77" s="75">
         <v>0.88621000000000005</v>
       </c>
-      <c r="E77" s="116">
+      <c r="E77" s="122">
         <v>0.88625600000000004</v>
       </c>
-      <c r="F77" s="53">
+      <c r="F77" s="36">
         <v>0.87528799999999995</v>
       </c>
-      <c r="G77" s="77">
+      <c r="G77" s="51">
         <v>0.87279899999999999</v>
       </c>
       <c r="H77" s="1"/>
     </row>
     <row r="78" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A78" s="1"/>
-      <c r="B78" s="54" t="s">
+      <c r="B78" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="C78" s="55" t="s">
+      <c r="C78" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="D78" s="107">
+      <c r="D78" s="70">
         <v>0.85210200000000003</v>
       </c>
-      <c r="E78" s="79">
+      <c r="E78" s="115">
         <v>0.85212500000000002</v>
       </c>
-      <c r="F78" s="80">
+      <c r="F78" s="54">
         <v>0.98280900000000004</v>
       </c>
-      <c r="G78" s="79">
+      <c r="G78" s="53">
         <v>0.98273900000000003</v>
       </c>
       <c r="H78" s="1"/>
     </row>
     <row r="79" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
-      <c r="B79" s="56"/>
-      <c r="C79" s="57" t="s">
+      <c r="B79" s="81"/>
+      <c r="C79" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="D79" s="108">
+      <c r="D79" s="71">
         <v>0.85321199999999997</v>
       </c>
-      <c r="E79" s="82">
+      <c r="E79" s="116">
         <v>0.853074</v>
       </c>
-      <c r="F79" s="83">
+      <c r="F79" s="57">
         <v>0.84496199999999999</v>
       </c>
-      <c r="G79" s="82">
+      <c r="G79" s="56">
         <v>0.83864799999999995</v>
       </c>
       <c r="H79" s="1"/>
     </row>
     <row r="80" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A80" s="1"/>
-      <c r="B80" s="48" t="s">
+      <c r="B80" s="78" t="s">
         <v>24</v>
       </c>
-      <c r="C80" s="49" t="s">
+      <c r="C80" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="D80" s="117">
+      <c r="D80" s="76">
         <v>0.90964299999999998</v>
       </c>
-      <c r="E80" s="84">
+      <c r="E80" s="126">
         <v>0.90964299999999998</v>
       </c>
-      <c r="F80" s="85">
+      <c r="F80" s="59">
         <v>0.98596600000000001</v>
       </c>
-      <c r="G80" s="84">
+      <c r="G80" s="58">
         <v>0.98596600000000001</v>
       </c>
       <c r="H80" s="1"/>
     </row>
     <row r="81" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
-      <c r="B81" s="46"/>
-      <c r="C81" s="47" t="s">
+      <c r="B81" s="79"/>
+      <c r="C81" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="D81" s="118">
+      <c r="D81" s="77">
         <v>0.91519899999999998</v>
       </c>
-      <c r="E81" s="86">
+      <c r="E81" s="127">
         <v>0.91519899999999998</v>
       </c>
-      <c r="F81" s="87">
+      <c r="F81" s="60">
         <v>0.906304</v>
       </c>
-      <c r="G81" s="111">
+      <c r="G81" s="74">
         <v>0.90293999999999996</v>
       </c>
       <c r="H81" s="1"/>
@@ -3154,8 +3223,10 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" s="1"/>
-      <c r="B83" s="1"/>
-      <c r="C83" s="1"/>
+      <c r="B83" s="111"/>
+      <c r="C83" s="19" t="s">
+        <v>31</v>
+      </c>
       <c r="D83" s="1"/>
       <c r="E83" s="1"/>
       <c r="F83" s="1"/>
@@ -3165,7 +3236,7 @@
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
-      <c r="C84" s="1"/>
+      <c r="C84" s="19"/>
       <c r="D84" s="1"/>
       <c r="E84" s="1"/>
       <c r="F84" s="1"/>
@@ -3173,47 +3244,97 @@
       <c r="H84" s="1"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B85" s="1"/>
-      <c r="C85" s="1"/>
+      <c r="A85" s="1"/>
+      <c r="B85" s="112"/>
+      <c r="C85" s="19" t="s">
+        <v>32</v>
+      </c>
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
       <c r="F85" s="1"/>
       <c r="G85" s="1"/>
+      <c r="H85" s="1"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A86" s="1"/>
+      <c r="B86" s="1"/>
+      <c r="C86" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D86" s="1"/>
+      <c r="E86" s="1"/>
+      <c r="F86" s="1"/>
+      <c r="G86" s="1"/>
+      <c r="H86" s="1"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A87" s="1"/>
+      <c r="B87" s="1"/>
+      <c r="C87" s="1"/>
+      <c r="D87" s="1"/>
+      <c r="E87" s="1"/>
+      <c r="F87" s="1"/>
+      <c r="G87" s="1"/>
+      <c r="H87" s="1"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A88" s="1"/>
+      <c r="B88" s="1"/>
+      <c r="C88" s="1"/>
+      <c r="D88" s="1"/>
+      <c r="E88" s="1"/>
+      <c r="F88" s="1"/>
+      <c r="G88" s="1"/>
+      <c r="H88" s="1"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A89" s="1"/>
+      <c r="B89" s="1"/>
+      <c r="C89" s="1"/>
+      <c r="D89" s="1"/>
+      <c r="E89" s="1"/>
+      <c r="F89" s="1"/>
+      <c r="G89" s="1"/>
+      <c r="H89" s="1"/>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A90" s="1"/>
+      <c r="B90" s="1"/>
+      <c r="C90" s="1"/>
+      <c r="D90" s="1"/>
+      <c r="E90" s="1"/>
+      <c r="F90" s="1"/>
+      <c r="G90" s="1"/>
+      <c r="H90" s="1"/>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A91" s="1"/>
+      <c r="B91" s="1"/>
+      <c r="C91" s="1"/>
+      <c r="D91" s="1"/>
+      <c r="E91" s="1"/>
+      <c r="F91" s="1"/>
+      <c r="G91" s="1"/>
+      <c r="H91" s="1"/>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A92" s="1"/>
+      <c r="B92" s="1"/>
+      <c r="C92" s="1"/>
+      <c r="D92" s="1"/>
+      <c r="E92" s="1"/>
+      <c r="F92" s="1"/>
+      <c r="G92" s="1"/>
+      <c r="H92" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="B80:B81"/>
-    <mergeCell ref="B72:B73"/>
-    <mergeCell ref="B74:B75"/>
-    <mergeCell ref="B76:B77"/>
-    <mergeCell ref="B78:B79"/>
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="B66:B67"/>
-    <mergeCell ref="B68:B69"/>
-    <mergeCell ref="B70:B71"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="B32:C33"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="B52:C53"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B18:C19"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="F22:G23"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B25:C26"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F20:G21"/>
+    <mergeCell ref="B20:B21"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="F4:G4"/>
@@ -3225,12 +3346,38 @@
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="H11:I11"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B25:C26"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F20:G21"/>
-    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B18:C19"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="F22:G23"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="B52:C53"/>
+    <mergeCell ref="B32:C33"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="B66:B67"/>
+    <mergeCell ref="B68:B69"/>
+    <mergeCell ref="B70:B71"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="B80:B81"/>
+    <mergeCell ref="B72:B73"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="B76:B77"/>
+    <mergeCell ref="B78:B79"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
website screenshots for readme
</commit_message>
<xml_diff>
--- a/Project_info/Summery tables for report.xlsx
+++ b/Project_info/Summery tables for report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sylviabroadbent/Dropbox/Sylvia/UWA_Data_Analytics_Bootcamp/HOMEWORK/23 Project 3/Data-Analytics-Project-3/Project_info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D39F137-D515-1B4C-9EC6-06225D609636}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DB8A706-E246-5F45-BC8B-9DFA09BDD8EE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25940" yWindow="-260" windowWidth="25600" windowHeight="28300" xr2:uid="{0BBD23A4-A283-624D-B6D4-A1A16531C452}"/>
+    <workbookView xWindow="12880" yWindow="500" windowWidth="25600" windowHeight="28300" xr2:uid="{0BBD23A4-A283-624D-B6D4-A1A16531C452}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="43">
   <si>
     <t>SMOKING</t>
   </si>
@@ -135,7 +135,34 @@
     <t>Models used for the website based on Github file size limit</t>
   </si>
   <si>
-    <t>&amp; because I ddin't save the RAW model</t>
+    <t>Model 1</t>
+  </si>
+  <si>
+    <t>Model 2</t>
+  </si>
+  <si>
+    <t>Model 3</t>
+  </si>
+  <si>
+    <t>Model 4</t>
+  </si>
+  <si>
+    <t>Hidden nodes</t>
+  </si>
+  <si>
+    <t>middle layers</t>
+  </si>
+  <si>
+    <t>Dataset</t>
+  </si>
+  <si>
+    <t>SEQUENTIAL</t>
+  </si>
+  <si>
+    <t>VALIDATION</t>
+  </si>
+  <si>
+    <t>&amp; because I didn't save the RAW model</t>
   </si>
 </sst>
 </file>
@@ -194,7 +221,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="73">
+  <borders count="87">
     <border>
       <left/>
       <right/>
@@ -1134,11 +1161,187 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF003B46"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF003B46"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF003B46"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF003B46"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF003B46"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF003B46"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF003B46"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF003B46"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF003B46"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF003B46"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF003B46"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF003B46"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF003B46"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF003B46"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF003B46"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF003B46"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="147">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1231,105 +1434,6 @@
     <xf numFmtId="164" fontId="1" fillId="2" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="70" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="70" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1347,6 +1451,144 @@
     <xf numFmtId="164" fontId="1" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="86" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1355,8 +1597,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF003B46"/>
       <color rgb="FFCCEBF0"/>
-      <color rgb="FF003B46"/>
       <color rgb="FF00AAEA"/>
       <color rgb="FF013C7F"/>
     </mruColors>
@@ -1669,18 +1911,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA521345-460E-3447-B7BC-D9B25ACFAE5B}">
-  <dimension ref="A3:L92"/>
+  <dimension ref="A3:R92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="L83" sqref="L83"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="E87" sqref="E87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1694,30 +1939,30 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
-      <c r="B4" s="86" t="s">
+      <c r="B4" s="97" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="87"/>
-      <c r="D4" s="90" t="s">
+      <c r="C4" s="98"/>
+      <c r="D4" s="101" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="91"/>
-      <c r="F4" s="92" t="s">
+      <c r="E4" s="102"/>
+      <c r="F4" s="103" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="92"/>
-      <c r="H4" s="90" t="s">
+      <c r="G4" s="103"/>
+      <c r="H4" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="91"/>
+      <c r="I4" s="102"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="88"/>
-      <c r="C5" s="89"/>
+      <c r="B5" s="99"/>
+      <c r="C5" s="100"/>
       <c r="D5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1738,9 +1983,9 @@
       </c>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
-      <c r="B6" s="93" t="s">
+      <c r="B6" s="95" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -1765,10 +2010,18 @@
         <v>0.60183200000000003</v>
       </c>
       <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+    </row>
+    <row r="7" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="94"/>
+      <c r="B7" s="108"/>
       <c r="C7" s="10" t="s">
         <v>6</v>
       </c>
@@ -1791,10 +2044,18 @@
         <v>0.59632200000000002</v>
       </c>
       <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="1:12" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+    </row>
+    <row r="8" spans="1:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="93" t="s">
+      <c r="B8" s="95" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="6" t="s">
@@ -1819,10 +2080,18 @@
         <v>0.79658899999999999</v>
       </c>
       <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+    </row>
+    <row r="9" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="95"/>
+      <c r="B9" s="96"/>
       <c r="C9" s="15" t="s">
         <v>6</v>
       </c>
@@ -1845,8 +2114,28 @@
         <v>0.57438400000000001</v>
       </c>
       <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K9" s="1"/>
+      <c r="L9" s="128" t="s">
+        <v>40</v>
+      </c>
+      <c r="M9" s="130" t="s">
+        <v>39</v>
+      </c>
+      <c r="N9" s="132" t="s">
+        <v>33</v>
+      </c>
+      <c r="O9" s="137" t="s">
+        <v>34</v>
+      </c>
+      <c r="P9" s="132" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q9" s="142" t="s">
+        <v>36</v>
+      </c>
+      <c r="R9" s="1"/>
+    </row>
+    <row r="10" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="19"/>
       <c r="C10" s="19"/>
@@ -1857,31 +2146,67 @@
       <c r="H10" s="19"/>
       <c r="I10" s="19"/>
       <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K10" s="1"/>
+      <c r="L10" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="M10" s="6"/>
+      <c r="N10" s="133">
+        <v>6</v>
+      </c>
+      <c r="O10" s="138">
+        <v>6</v>
+      </c>
+      <c r="P10" s="133">
+        <v>15</v>
+      </c>
+      <c r="Q10" s="143">
+        <v>15</v>
+      </c>
+      <c r="R10" s="1"/>
+    </row>
+    <row r="11" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="B11" s="86" t="s">
+      <c r="B11" s="97" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="87"/>
-      <c r="D11" s="90" t="s">
+      <c r="C11" s="98"/>
+      <c r="D11" s="101" t="s">
         <v>1</v>
       </c>
-      <c r="E11" s="91"/>
-      <c r="F11" s="92" t="s">
+      <c r="E11" s="102"/>
+      <c r="F11" s="103" t="s">
         <v>2</v>
       </c>
-      <c r="G11" s="92"/>
-      <c r="H11" s="90" t="s">
+      <c r="G11" s="103"/>
+      <c r="H11" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="I11" s="91"/>
+      <c r="I11" s="102"/>
       <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K11" s="1"/>
+      <c r="L11" s="129" t="s">
+        <v>38</v>
+      </c>
+      <c r="M11" s="131"/>
+      <c r="N11" s="134">
+        <v>1</v>
+      </c>
+      <c r="O11" s="139">
+        <v>2</v>
+      </c>
+      <c r="P11" s="134">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="144">
+        <v>2</v>
+      </c>
+      <c r="R11" s="1"/>
+    </row>
+    <row r="12" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="88"/>
-      <c r="C12" s="89"/>
+      <c r="B12" s="99"/>
+      <c r="C12" s="100"/>
       <c r="D12" s="2" t="s">
         <v>7</v>
       </c>
@@ -1901,10 +2226,28 @@
         <v>8</v>
       </c>
       <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K12" s="1"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="N12" s="135">
+        <v>0.37943500000000002</v>
+      </c>
+      <c r="O12" s="140">
+        <v>0.37609999999999999</v>
+      </c>
+      <c r="P12" s="135">
+        <v>0.37530000000000002</v>
+      </c>
+      <c r="Q12" s="145">
+        <v>0.37630000000000002</v>
+      </c>
+      <c r="R12" s="1"/>
+    </row>
+    <row r="13" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="B13" s="93" t="s">
+      <c r="B13" s="95" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="6" t="s">
@@ -1929,10 +2272,28 @@
         <v>0.37883299999999998</v>
       </c>
       <c r="J13" s="1"/>
-    </row>
-    <row r="14" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K13" s="1"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="N13" s="136">
+        <v>0.37685600000000002</v>
+      </c>
+      <c r="O13" s="141">
+        <v>0.37909999999999999</v>
+      </c>
+      <c r="P13" s="136">
+        <v>0.37769999999999998</v>
+      </c>
+      <c r="Q13" s="146">
+        <v>0.37690000000000001</v>
+      </c>
+      <c r="R13" s="1"/>
+    </row>
+    <row r="14" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
-      <c r="B14" s="94"/>
+      <c r="B14" s="108"/>
       <c r="C14" s="10" t="s">
         <v>6</v>
       </c>
@@ -1955,10 +2316,18 @@
         <v>0.372614</v>
       </c>
       <c r="J14" s="1"/>
-    </row>
-    <row r="15" spans="1:12" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+    </row>
+    <row r="15" spans="1:18" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
-      <c r="B15" s="93" t="s">
+      <c r="B15" s="95" t="s">
         <v>4</v>
       </c>
       <c r="C15" s="6" t="s">
@@ -1983,10 +2352,18 @@
         <v>0.87316499999999997</v>
       </c>
       <c r="J15" s="1"/>
-    </row>
-    <row r="16" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+    </row>
+    <row r="16" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="95"/>
+      <c r="B16" s="96"/>
       <c r="C16" s="15" t="s">
         <v>6</v>
       </c>
@@ -2009,6 +2386,14 @@
         <v>0.47225499999999998</v>
       </c>
       <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
     </row>
     <row r="17" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
@@ -2024,28 +2409,28 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
-      <c r="B18" s="86" t="s">
+      <c r="B18" s="97" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="87"/>
-      <c r="D18" s="90" t="s">
+      <c r="C18" s="98"/>
+      <c r="D18" s="101" t="s">
         <v>1</v>
       </c>
-      <c r="E18" s="91"/>
-      <c r="F18" s="92" t="s">
+      <c r="E18" s="102"/>
+      <c r="F18" s="103" t="s">
         <v>2</v>
       </c>
-      <c r="G18" s="92"/>
-      <c r="H18" s="90" t="s">
+      <c r="G18" s="103"/>
+      <c r="H18" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="I18" s="91"/>
+      <c r="I18" s="102"/>
       <c r="J18" s="1"/>
     </row>
     <row r="19" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="88"/>
-      <c r="C19" s="89"/>
+      <c r="B19" s="99"/>
+      <c r="C19" s="100"/>
       <c r="D19" s="2" t="s">
         <v>7</v>
       </c>
@@ -2068,7 +2453,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
-      <c r="B20" s="93" t="s">
+      <c r="B20" s="95" t="s">
         <v>11</v>
       </c>
       <c r="C20" s="6" t="s">
@@ -2080,10 +2465,10 @@
       <c r="E20" s="8">
         <v>0.92258300000000004</v>
       </c>
-      <c r="F20" s="107" t="s">
+      <c r="F20" s="104" t="s">
         <v>12</v>
       </c>
-      <c r="G20" s="108"/>
+      <c r="G20" s="105"/>
       <c r="H20" s="7">
         <v>0.922018</v>
       </c>
@@ -2094,7 +2479,7 @@
     </row>
     <row r="21" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
-      <c r="B21" s="94"/>
+      <c r="B21" s="108"/>
       <c r="C21" s="10" t="s">
         <v>6</v>
       </c>
@@ -2104,8 +2489,8 @@
       <c r="E21" s="12">
         <v>0.92082200000000003</v>
       </c>
-      <c r="F21" s="109"/>
-      <c r="G21" s="110"/>
+      <c r="F21" s="106"/>
+      <c r="G21" s="107"/>
       <c r="H21" s="14">
         <v>0.91990000000000005</v>
       </c>
@@ -2116,7 +2501,7 @@
     </row>
     <row r="22" spans="1:11" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
-      <c r="B22" s="93" t="s">
+      <c r="B22" s="95" t="s">
         <v>4</v>
       </c>
       <c r="C22" s="6" t="s">
@@ -2128,10 +2513,10 @@
       <c r="E22" s="8">
         <v>0.99874399999999997</v>
       </c>
-      <c r="F22" s="103" t="s">
+      <c r="F22" s="109" t="s">
         <v>12</v>
       </c>
-      <c r="G22" s="104"/>
+      <c r="G22" s="110"/>
       <c r="H22" s="39">
         <v>0.99228000000000005</v>
       </c>
@@ -2142,7 +2527,7 @@
     </row>
     <row r="23" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="95"/>
+      <c r="B23" s="96"/>
       <c r="C23" s="15" t="s">
         <v>6</v>
       </c>
@@ -2152,8 +2537,8 @@
       <c r="E23" s="25">
         <v>0.91980799999999996</v>
       </c>
-      <c r="F23" s="105"/>
-      <c r="G23" s="106"/>
+      <c r="F23" s="111"/>
+      <c r="G23" s="112"/>
       <c r="H23" s="16">
         <v>0.91561400000000004</v>
       </c>
@@ -2176,29 +2561,29 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
-      <c r="B25" s="86" t="s">
+      <c r="B25" s="97" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="87"/>
-      <c r="D25" s="90" t="s">
+      <c r="C25" s="98"/>
+      <c r="D25" s="101" t="s">
         <v>27</v>
       </c>
-      <c r="E25" s="91"/>
-      <c r="F25" s="92" t="s">
+      <c r="E25" s="102"/>
+      <c r="F25" s="103" t="s">
         <v>15</v>
       </c>
-      <c r="G25" s="92"/>
-      <c r="H25" s="90" t="s">
+      <c r="G25" s="103"/>
+      <c r="H25" s="101" t="s">
         <v>28</v>
       </c>
-      <c r="I25" s="91"/>
+      <c r="I25" s="102"/>
       <c r="J25" s="45"/>
       <c r="K25" s="45"/>
     </row>
     <row r="26" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
-      <c r="B26" s="88"/>
-      <c r="C26" s="89"/>
+      <c r="B26" s="99"/>
+      <c r="C26" s="100"/>
       <c r="D26" s="2" t="s">
         <v>7</v>
       </c>
@@ -2222,7 +2607,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
-      <c r="B27" s="93" t="s">
+      <c r="B27" s="95" t="s">
         <v>11</v>
       </c>
       <c r="C27" s="6" t="s">
@@ -2251,7 +2636,7 @@
     </row>
     <row r="28" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
-      <c r="B28" s="94"/>
+      <c r="B28" s="108"/>
       <c r="C28" s="10" t="s">
         <v>6</v>
       </c>
@@ -2278,7 +2663,7 @@
     </row>
     <row r="29" spans="1:11" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
-      <c r="B29" s="93" t="s">
+      <c r="B29" s="95" t="s">
         <v>4</v>
       </c>
       <c r="C29" s="6" t="s">
@@ -2307,7 +2692,7 @@
     </row>
     <row r="30" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
-      <c r="B30" s="95"/>
+      <c r="B30" s="96"/>
       <c r="C30" s="15" t="s">
         <v>6</v>
       </c>
@@ -2347,28 +2732,28 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
-      <c r="B32" s="86" t="s">
+      <c r="B32" s="97" t="s">
         <v>26</v>
       </c>
-      <c r="C32" s="87"/>
-      <c r="D32" s="90" t="s">
+      <c r="C32" s="98"/>
+      <c r="D32" s="101" t="s">
         <v>27</v>
       </c>
-      <c r="E32" s="91"/>
-      <c r="F32" s="92" t="s">
+      <c r="E32" s="102"/>
+      <c r="F32" s="103" t="s">
         <v>15</v>
       </c>
-      <c r="G32" s="92"/>
-      <c r="H32" s="90" t="s">
+      <c r="G32" s="103"/>
+      <c r="H32" s="101" t="s">
         <v>29</v>
       </c>
-      <c r="I32" s="91"/>
+      <c r="I32" s="102"/>
       <c r="J32" s="1"/>
     </row>
     <row r="33" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
-      <c r="B33" s="88"/>
-      <c r="C33" s="89"/>
+      <c r="B33" s="99"/>
+      <c r="C33" s="100"/>
       <c r="D33" s="2" t="s">
         <v>7</v>
       </c>
@@ -2391,7 +2776,7 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
-      <c r="B34" s="93" t="s">
+      <c r="B34" s="95" t="s">
         <v>11</v>
       </c>
       <c r="C34" s="6" t="s">
@@ -2419,7 +2804,7 @@
     </row>
     <row r="35" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
-      <c r="B35" s="94"/>
+      <c r="B35" s="108"/>
       <c r="C35" s="10" t="s">
         <v>6</v>
       </c>
@@ -2445,7 +2830,7 @@
     </row>
     <row r="36" spans="1:12" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
-      <c r="B36" s="93" t="s">
+      <c r="B36" s="95" t="s">
         <v>4</v>
       </c>
       <c r="C36" s="6" t="s">
@@ -2473,14 +2858,14 @@
     </row>
     <row r="37" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
-      <c r="B37" s="95"/>
+      <c r="B37" s="96"/>
       <c r="C37" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D37" s="113">
+      <c r="D37" s="80">
         <v>0.71919</v>
       </c>
-      <c r="E37" s="114">
+      <c r="E37" s="81">
         <v>0.71389000000000002</v>
       </c>
       <c r="F37" s="24">
@@ -2511,28 +2896,46 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
       <c r="J41" s="1"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
       <c r="J42" s="1"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
       <c r="J43" s="1"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
       <c r="J44" s="30"/>
       <c r="K44" s="30"/>
     </row>
@@ -2588,24 +2991,24 @@
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" s="30"/>
-      <c r="B52" s="96" t="s">
+      <c r="B52" s="123" t="s">
         <v>13</v>
       </c>
-      <c r="C52" s="97"/>
-      <c r="D52" s="99" t="s">
+      <c r="C52" s="124"/>
+      <c r="D52" s="113" t="s">
         <v>11</v>
       </c>
-      <c r="E52" s="100"/>
-      <c r="F52" s="101" t="s">
+      <c r="E52" s="114"/>
+      <c r="F52" s="115" t="s">
         <v>4</v>
       </c>
-      <c r="G52" s="102"/>
+      <c r="G52" s="116"/>
       <c r="H52" s="1"/>
     </row>
     <row r="53" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="30"/>
-      <c r="B53" s="98"/>
-      <c r="C53" s="89"/>
+      <c r="B53" s="125"/>
+      <c r="C53" s="100"/>
       <c r="D53" s="2" t="s">
         <v>7</v>
       </c>
@@ -2622,7 +3025,7 @@
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" s="30"/>
-      <c r="B54" s="82" t="s">
+      <c r="B54" s="117" t="s">
         <v>0</v>
       </c>
       <c r="C54" s="6" t="s">
@@ -2631,7 +3034,7 @@
       <c r="D54" s="65">
         <v>0.99935399999999996</v>
       </c>
-      <c r="E54" s="119">
+      <c r="E54" s="86">
         <v>0.99935399999999996</v>
       </c>
       <c r="F54" s="7">
@@ -2644,14 +3047,14 @@
     </row>
     <row r="55" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" s="30"/>
-      <c r="B55" s="83"/>
+      <c r="B55" s="118"/>
       <c r="C55" s="10" t="s">
         <v>6</v>
       </c>
       <c r="D55" s="66">
         <v>0.99939999999999996</v>
       </c>
-      <c r="E55" s="125">
+      <c r="E55" s="92">
         <v>0.99939999999999996</v>
       </c>
       <c r="F55" s="34">
@@ -2664,16 +3067,16 @@
     </row>
     <row r="56" spans="1:12" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A56" s="30"/>
-      <c r="B56" s="84" t="s">
+      <c r="B56" s="119" t="s">
         <v>9</v>
       </c>
       <c r="C56" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D56" s="123">
+      <c r="D56" s="90">
         <v>0.378361</v>
       </c>
-      <c r="E56" s="121">
+      <c r="E56" s="88">
         <v>0.37816499999999997</v>
       </c>
       <c r="F56" s="29">
@@ -2689,14 +3092,14 @@
     </row>
     <row r="57" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A57" s="30"/>
-      <c r="B57" s="85"/>
+      <c r="B57" s="120"/>
       <c r="C57" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="D57" s="124">
+      <c r="D57" s="91">
         <v>0.37238399999999999</v>
       </c>
-      <c r="E57" s="122">
+      <c r="E57" s="89">
         <v>0.37196899999999999</v>
       </c>
       <c r="F57" s="36">
@@ -2709,7 +3112,7 @@
     </row>
     <row r="58" spans="1:12" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A58" s="30"/>
-      <c r="B58" s="80" t="s">
+      <c r="B58" s="121" t="s">
         <v>10</v>
       </c>
       <c r="C58" s="37" t="s">
@@ -2718,7 +3121,7 @@
       <c r="D58" s="52">
         <v>0.92019799999999996</v>
       </c>
-      <c r="E58" s="115">
+      <c r="E58" s="82">
         <v>0.92040500000000003</v>
       </c>
       <c r="F58" s="54">
@@ -2731,14 +3134,14 @@
     </row>
     <row r="59" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="30"/>
-      <c r="B59" s="81"/>
+      <c r="B59" s="122"/>
       <c r="C59" s="38" t="s">
         <v>6</v>
       </c>
       <c r="D59" s="61">
         <v>0.91754999999999998</v>
       </c>
-      <c r="E59" s="116">
+      <c r="E59" s="83">
         <v>0.91773400000000005</v>
       </c>
       <c r="F59" s="57">
@@ -2751,7 +3154,7 @@
     </row>
     <row r="60" spans="1:12" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A60" s="30"/>
-      <c r="B60" s="80" t="s">
+      <c r="B60" s="121" t="s">
         <v>14</v>
       </c>
       <c r="C60" s="37" t="s">
@@ -2760,7 +3163,7 @@
       <c r="D60" s="52">
         <v>0.72340099999999996</v>
       </c>
-      <c r="E60" s="115">
+      <c r="E60" s="82">
         <v>0.72335499999999997</v>
       </c>
       <c r="F60" s="54">
@@ -2773,14 +3176,14 @@
     </row>
     <row r="61" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A61" s="30"/>
-      <c r="B61" s="81"/>
+      <c r="B61" s="122"/>
       <c r="C61" s="38" t="s">
         <v>6</v>
       </c>
       <c r="D61" s="55">
         <v>0.72089499999999995</v>
       </c>
-      <c r="E61" s="116">
+      <c r="E61" s="83">
         <v>0.72117200000000004</v>
       </c>
       <c r="F61" s="69">
@@ -2793,7 +3196,7 @@
     </row>
     <row r="62" spans="1:12" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A62" s="30"/>
-      <c r="B62" s="80" t="s">
+      <c r="B62" s="121" t="s">
         <v>15</v>
       </c>
       <c r="C62" s="37" t="s">
@@ -2802,7 +3205,7 @@
       <c r="D62" s="70">
         <v>0.887602</v>
       </c>
-      <c r="E62" s="117">
+      <c r="E62" s="84">
         <v>0.887602</v>
       </c>
       <c r="F62" s="54">
@@ -2815,14 +3218,14 @@
     </row>
     <row r="63" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A63" s="30"/>
-      <c r="B63" s="81"/>
+      <c r="B63" s="122"/>
       <c r="C63" s="38" t="s">
         <v>6</v>
       </c>
       <c r="D63" s="71">
         <v>0.890266</v>
       </c>
-      <c r="E63" s="118">
+      <c r="E63" s="85">
         <v>0.890266</v>
       </c>
       <c r="F63" s="57">
@@ -2835,7 +3238,7 @@
     </row>
     <row r="64" spans="1:12" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A64" s="30"/>
-      <c r="B64" s="82" t="s">
+      <c r="B64" s="117" t="s">
         <v>16</v>
       </c>
       <c r="C64" s="6" t="s">
@@ -2844,7 +3247,7 @@
       <c r="D64" s="7">
         <v>0.98300399999999999</v>
       </c>
-      <c r="E64" s="119">
+      <c r="E64" s="86">
         <v>0.98300399999999999</v>
       </c>
       <c r="F64" s="72">
@@ -2857,14 +3260,14 @@
     </row>
     <row r="65" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
-      <c r="B65" s="83"/>
+      <c r="B65" s="118"/>
       <c r="C65" s="10" t="s">
         <v>6</v>
       </c>
       <c r="D65" s="11">
         <v>0.98391499999999998</v>
       </c>
-      <c r="E65" s="120">
+      <c r="E65" s="87">
         <v>0.98391499999999998</v>
       </c>
       <c r="F65" s="73">
@@ -2877,7 +3280,7 @@
     </row>
     <row r="66" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1"/>
-      <c r="B66" s="84" t="s">
+      <c r="B66" s="119" t="s">
         <v>17</v>
       </c>
       <c r="C66" s="27" t="s">
@@ -2886,7 +3289,7 @@
       <c r="D66" s="28">
         <v>0.99142699999999995</v>
       </c>
-      <c r="E66" s="121">
+      <c r="E66" s="88">
         <v>0.99142699999999995</v>
       </c>
       <c r="F66" s="67">
@@ -2899,14 +3302,14 @@
     </row>
     <row r="67" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
-      <c r="B67" s="85"/>
+      <c r="B67" s="120"/>
       <c r="C67" s="33" t="s">
         <v>6</v>
       </c>
       <c r="D67" s="34">
         <v>0.991842</v>
       </c>
-      <c r="E67" s="122">
+      <c r="E67" s="89">
         <v>0.991842</v>
       </c>
       <c r="F67" s="68">
@@ -2919,7 +3322,7 @@
     </row>
     <row r="68" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1"/>
-      <c r="B68" s="80" t="s">
+      <c r="B68" s="121" t="s">
         <v>18</v>
       </c>
       <c r="C68" s="37" t="s">
@@ -2928,7 +3331,7 @@
       <c r="D68" s="70">
         <v>0.96610200000000002</v>
       </c>
-      <c r="E68" s="115">
+      <c r="E68" s="82">
         <v>0.96610200000000002</v>
       </c>
       <c r="F68" s="54">
@@ -2941,14 +3344,14 @@
     </row>
     <row r="69" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
-      <c r="B69" s="81"/>
+      <c r="B69" s="122"/>
       <c r="C69" s="38" t="s">
         <v>6</v>
       </c>
       <c r="D69" s="71">
         <v>0.96644799999999997</v>
       </c>
-      <c r="E69" s="116">
+      <c r="E69" s="83">
         <v>0.96644799999999997</v>
       </c>
       <c r="F69" s="69">
@@ -2961,7 +3364,7 @@
     </row>
     <row r="70" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1"/>
-      <c r="B70" s="80" t="s">
+      <c r="B70" s="121" t="s">
         <v>19</v>
       </c>
       <c r="C70" s="37" t="s">
@@ -2970,7 +3373,7 @@
       <c r="D70" s="70">
         <v>0.66734599999999999</v>
       </c>
-      <c r="E70" s="115">
+      <c r="E70" s="82">
         <v>0.66751899999999997</v>
       </c>
       <c r="F70" s="54">
@@ -2983,14 +3386,14 @@
     </row>
     <row r="71" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
-      <c r="B71" s="81"/>
+      <c r="B71" s="122"/>
       <c r="C71" s="38" t="s">
         <v>6</v>
       </c>
       <c r="D71" s="71">
         <v>0.66522199999999998</v>
       </c>
-      <c r="E71" s="116">
+      <c r="E71" s="83">
         <v>0.66448499999999999</v>
       </c>
       <c r="F71" s="69">
@@ -3003,7 +3406,7 @@
     </row>
     <row r="72" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A72" s="1"/>
-      <c r="B72" s="80" t="s">
+      <c r="B72" s="121" t="s">
         <v>20</v>
       </c>
       <c r="C72" s="37" t="s">
@@ -3012,7 +3415,7 @@
       <c r="D72" s="70">
         <v>0.80465399999999998</v>
       </c>
-      <c r="E72" s="115">
+      <c r="E72" s="82">
         <v>0.80290300000000003</v>
       </c>
       <c r="F72" s="54">
@@ -3025,14 +3428,14 @@
     </row>
     <row r="73" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
-      <c r="B73" s="81"/>
+      <c r="B73" s="122"/>
       <c r="C73" s="38" t="s">
         <v>6</v>
       </c>
       <c r="D73" s="71">
         <v>0.80680200000000002</v>
       </c>
-      <c r="E73" s="116">
+      <c r="E73" s="83">
         <v>0.80495799999999995</v>
       </c>
       <c r="F73" s="57">
@@ -3045,7 +3448,7 @@
     </row>
     <row r="74" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A74" s="1"/>
-      <c r="B74" s="82" t="s">
+      <c r="B74" s="117" t="s">
         <v>21</v>
       </c>
       <c r="C74" s="6" t="s">
@@ -3054,7 +3457,7 @@
       <c r="D74" s="39">
         <v>0.86419999999999997</v>
       </c>
-      <c r="E74" s="119">
+      <c r="E74" s="86">
         <v>0.86431599999999997</v>
       </c>
       <c r="F74" s="26">
@@ -3067,14 +3470,14 @@
     </row>
     <row r="75" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
-      <c r="B75" s="83"/>
+      <c r="B75" s="118"/>
       <c r="C75" s="10" t="s">
         <v>6</v>
       </c>
       <c r="D75" s="11">
         <v>0.86630099999999999</v>
       </c>
-      <c r="E75" s="120">
+      <c r="E75" s="87">
         <v>0.86666900000000002</v>
       </c>
       <c r="F75" s="20">
@@ -3087,7 +3490,7 @@
     </row>
     <row r="76" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A76" s="1"/>
-      <c r="B76" s="84" t="s">
+      <c r="B76" s="119" t="s">
         <v>22</v>
       </c>
       <c r="C76" s="27" t="s">
@@ -3096,7 +3499,7 @@
       <c r="D76" s="28">
         <v>0.88769399999999998</v>
       </c>
-      <c r="E76" s="121">
+      <c r="E76" s="88">
         <v>0.88771699999999998</v>
       </c>
       <c r="F76" s="29">
@@ -3109,14 +3512,14 @@
     </row>
     <row r="77" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
-      <c r="B77" s="85"/>
+      <c r="B77" s="120"/>
       <c r="C77" s="33" t="s">
         <v>6</v>
       </c>
       <c r="D77" s="75">
         <v>0.88621000000000005</v>
       </c>
-      <c r="E77" s="122">
+      <c r="E77" s="89">
         <v>0.88625600000000004</v>
       </c>
       <c r="F77" s="36">
@@ -3129,7 +3532,7 @@
     </row>
     <row r="78" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A78" s="1"/>
-      <c r="B78" s="80" t="s">
+      <c r="B78" s="121" t="s">
         <v>23</v>
       </c>
       <c r="C78" s="37" t="s">
@@ -3138,7 +3541,7 @@
       <c r="D78" s="70">
         <v>0.85210200000000003</v>
       </c>
-      <c r="E78" s="115">
+      <c r="E78" s="82">
         <v>0.85212500000000002</v>
       </c>
       <c r="F78" s="54">
@@ -3151,14 +3554,14 @@
     </row>
     <row r="79" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
-      <c r="B79" s="81"/>
+      <c r="B79" s="122"/>
       <c r="C79" s="38" t="s">
         <v>6</v>
       </c>
       <c r="D79" s="71">
         <v>0.85321199999999997</v>
       </c>
-      <c r="E79" s="116">
+      <c r="E79" s="83">
         <v>0.853074</v>
       </c>
       <c r="F79" s="57">
@@ -3171,7 +3574,7 @@
     </row>
     <row r="80" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A80" s="1"/>
-      <c r="B80" s="78" t="s">
+      <c r="B80" s="126" t="s">
         <v>24</v>
       </c>
       <c r="C80" s="32" t="s">
@@ -3180,7 +3583,7 @@
       <c r="D80" s="76">
         <v>0.90964299999999998</v>
       </c>
-      <c r="E80" s="126">
+      <c r="E80" s="93">
         <v>0.90964299999999998</v>
       </c>
       <c r="F80" s="59">
@@ -3193,14 +3596,14 @@
     </row>
     <row r="81" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
-      <c r="B81" s="79"/>
+      <c r="B81" s="127"/>
       <c r="C81" s="31" t="s">
         <v>6</v>
       </c>
       <c r="D81" s="77">
         <v>0.91519899999999998</v>
       </c>
-      <c r="E81" s="127">
+      <c r="E81" s="94">
         <v>0.91519899999999998</v>
       </c>
       <c r="F81" s="60">
@@ -3223,7 +3626,7 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" s="1"/>
-      <c r="B83" s="111"/>
+      <c r="B83" s="78"/>
       <c r="C83" s="19" t="s">
         <v>31</v>
       </c>
@@ -3245,7 +3648,7 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" s="1"/>
-      <c r="B85" s="112"/>
+      <c r="B85" s="79"/>
       <c r="C85" s="19" t="s">
         <v>32</v>
       </c>
@@ -3259,7 +3662,7 @@
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="19" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
@@ -3329,12 +3732,35 @@
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B25:C26"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F20:G21"/>
-    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B80:B81"/>
+    <mergeCell ref="B72:B73"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="B76:B77"/>
+    <mergeCell ref="B78:B79"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="B66:B67"/>
+    <mergeCell ref="B68:B69"/>
+    <mergeCell ref="B70:B71"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="B52:C53"/>
+    <mergeCell ref="B32:C33"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="F22:G23"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="H32:I32"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="F4:G4"/>
@@ -3346,38 +3772,15 @@
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="H11:I11"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B25:C26"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F20:G21"/>
+    <mergeCell ref="B20:B21"/>
     <mergeCell ref="B18:C19"/>
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="F18:G18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="F22:G23"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="B52:C53"/>
-    <mergeCell ref="B32:C33"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="B66:B67"/>
-    <mergeCell ref="B68:B69"/>
-    <mergeCell ref="B70:B71"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="B80:B81"/>
-    <mergeCell ref="B72:B73"/>
-    <mergeCell ref="B74:B75"/>
-    <mergeCell ref="B76:B77"/>
-    <mergeCell ref="B78:B79"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>